<commit_message>
Update division names in Excel workbook to match actual divisions
Replaced sample division names with real organizational divisions:
- Marketing → Group Functions
- Sales → GWM (Global Wealth Management)
- Engineering → IB (Investment Banking)

Changes applied across all 5 worksheets:
- Employee data rows
- Step-by-step examples
- Business question text
- Filter descriptions
- Summary comparisons
- Sheet 3 renamed to "Division Filter (GrpFunc)"

All calculations and color coding remain intact.
Excel file ready for business stakeholder review with accurate division names.

🤖 Generated with [Claude Code](https://claude.com/claude-code)

Co-Authored-By: Claude <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/uv-aggregation-strategy/unique_reach_calculation_guide.xlsx
+++ b/uv-aggregation-strategy/unique_reach_calculation_guide.xlsx
@@ -9,7 +9,7 @@
   <sheets>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="1. Overview &amp; Sample Data" sheetId="1" state="visible" r:id="rId1"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="2. Site Filter (News&amp;Events)" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="3. Division Filter (Marketing)" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="3. Division Filter (GrpFunc)" sheetId="3" state="visible" r:id="rId3"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="4. Combined (Site+Division)" sheetId="4" state="visible" r:id="rId4"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="5. Summary &amp; Comparison" sheetId="5" state="visible" r:id="rId5"/>
   </sheets>
@@ -578,6 +578,7 @@
         </is>
       </c>
     </row>
+    <row r="2"/>
     <row r="3">
       <c r="A3" s="2" t="inlineStr">
         <is>
@@ -585,6 +586,7 @@
         </is>
       </c>
     </row>
+    <row r="4"/>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
@@ -602,17 +604,18 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>• Scenario 2: Division Filter - 'Marketing' (see Sheet 3)</t>
+          <t>• Scenario 2: Division Filter - 'Group Functions' (see Sheet 3)</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>• Scenario 3: Combined Filter - 'News &amp; Events' + 'Marketing' (see Sheet 4)</t>
-        </is>
-      </c>
-    </row>
+          <t>• Scenario 3: Combined Filter - 'News &amp; Events' + 'Group Functions' (see Sheet 4)</t>
+        </is>
+      </c>
+    </row>
+    <row r="9"/>
     <row r="10">
       <c r="A10" s="3" t="inlineStr">
         <is>
@@ -775,6 +778,7 @@
         </is>
       </c>
     </row>
+    <row r="15"/>
     <row r="16">
       <c r="A16" s="3" t="inlineStr">
         <is>
@@ -844,7 +848,7 @@
       </c>
       <c r="B18" s="7" t="inlineStr">
         <is>
-          <t>Marketing</t>
+          <t>Group Functions</t>
         </is>
       </c>
       <c r="C18" s="7" t="inlineStr">
@@ -891,7 +895,7 @@
       </c>
       <c r="B19" s="7" t="inlineStr">
         <is>
-          <t>Marketing</t>
+          <t>Group Functions</t>
         </is>
       </c>
       <c r="C19" s="7" t="inlineStr">
@@ -938,7 +942,7 @@
       </c>
       <c r="B20" s="7" t="inlineStr">
         <is>
-          <t>Sales</t>
+          <t>GWM</t>
         </is>
       </c>
       <c r="C20" s="7" t="inlineStr">
@@ -985,7 +989,7 @@
       </c>
       <c r="B21" s="7" t="inlineStr">
         <is>
-          <t>Marketing</t>
+          <t>Group Functions</t>
         </is>
       </c>
       <c r="C21" s="7" t="inlineStr">
@@ -1032,7 +1036,7 @@
       </c>
       <c r="B22" s="7" t="inlineStr">
         <is>
-          <t>Engineering</t>
+          <t>IB</t>
         </is>
       </c>
       <c r="C22" s="7" t="inlineStr">
@@ -1079,7 +1083,7 @@
       </c>
       <c r="B23" s="7" t="inlineStr">
         <is>
-          <t>Marketing</t>
+          <t>Group Functions</t>
         </is>
       </c>
       <c r="C23" s="7" t="inlineStr">
@@ -1184,6 +1188,7 @@
         </is>
       </c>
     </row>
+    <row r="3"/>
     <row r="4">
       <c r="A4" s="12" t="inlineStr">
         <is>
@@ -1261,7 +1266,7 @@
       </c>
       <c r="B6" s="7" t="inlineStr">
         <is>
-          <t>Marketing</t>
+          <t>Group Functions</t>
         </is>
       </c>
       <c r="C6" s="7" t="inlineStr">
@@ -1313,7 +1318,7 @@
       </c>
       <c r="B7" s="7" t="inlineStr">
         <is>
-          <t>Marketing</t>
+          <t>Group Functions</t>
         </is>
       </c>
       <c r="C7" s="7" t="inlineStr">
@@ -1365,7 +1370,7 @@
       </c>
       <c r="B8" s="7" t="inlineStr">
         <is>
-          <t>Sales</t>
+          <t>GWM</t>
         </is>
       </c>
       <c r="C8" s="7" t="inlineStr">
@@ -1417,7 +1422,7 @@
       </c>
       <c r="B9" s="7" t="inlineStr">
         <is>
-          <t>Marketing</t>
+          <t>Group Functions</t>
         </is>
       </c>
       <c r="C9" s="7" t="inlineStr">
@@ -1469,7 +1474,7 @@
       </c>
       <c r="B10" s="7" t="inlineStr">
         <is>
-          <t>Engineering</t>
+          <t>IB</t>
         </is>
       </c>
       <c r="C10" s="7" t="inlineStr">
@@ -1521,7 +1526,7 @@
       </c>
       <c r="B11" s="7" t="inlineStr">
         <is>
-          <t>Marketing</t>
+          <t>Group Functions</t>
         </is>
       </c>
       <c r="C11" s="7" t="inlineStr">
@@ -1565,6 +1570,7 @@
         </is>
       </c>
     </row>
+    <row r="12"/>
     <row r="13">
       <c r="A13" s="13" t="inlineStr">
         <is>
@@ -1632,7 +1638,7 @@
       </c>
       <c r="B15" s="7" t="inlineStr">
         <is>
-          <t>Marketing</t>
+          <t>Group Functions</t>
         </is>
       </c>
       <c r="C15" s="7" t="inlineStr">
@@ -1674,7 +1680,7 @@
       </c>
       <c r="B16" s="7" t="inlineStr">
         <is>
-          <t>Sales</t>
+          <t>GWM</t>
         </is>
       </c>
       <c r="C16" s="7" t="inlineStr">
@@ -1716,7 +1722,7 @@
       </c>
       <c r="B17" s="7" t="inlineStr">
         <is>
-          <t>Marketing</t>
+          <t>Group Functions</t>
         </is>
       </c>
       <c r="C17" s="7" t="inlineStr">
@@ -1758,7 +1764,7 @@
       </c>
       <c r="B18" s="7" t="inlineStr">
         <is>
-          <t>Engineering</t>
+          <t>IB</t>
         </is>
       </c>
       <c r="C18" s="7" t="inlineStr">
@@ -1800,7 +1806,7 @@
       </c>
       <c r="B19" s="7" t="inlineStr">
         <is>
-          <t>Marketing</t>
+          <t>Group Functions</t>
         </is>
       </c>
       <c r="C19" s="7" t="inlineStr">
@@ -1834,6 +1840,7 @@
         </is>
       </c>
     </row>
+    <row r="20"/>
     <row r="21">
       <c r="A21" s="14" t="inlineStr">
         <is>
@@ -2011,6 +2018,7 @@
         </is>
       </c>
     </row>
+    <row r="27"/>
     <row r="28">
       <c r="A28" s="16" t="inlineStr">
         <is>
@@ -2061,7 +2069,7 @@
     <row r="1">
       <c r="A1" s="10" t="inlineStr">
         <is>
-          <t>SCENARIO 2: Division Filter Only - 'Marketing'</t>
+          <t>SCENARIO 2: Division Filter Only - 'Group Functions'</t>
         </is>
       </c>
       <c r="B1" s="4" t="n"/>
@@ -2078,14 +2086,15 @@
     <row r="2">
       <c r="A2" s="11" t="inlineStr">
         <is>
-          <t>Business Question: What % of Marketing division engaged with ANY content?</t>
-        </is>
-      </c>
-    </row>
+          <t>Business Question: What % of Group Functions division engaged with ANY content?</t>
+        </is>
+      </c>
+    </row>
+    <row r="3"/>
     <row r="4">
       <c r="A4" s="12" t="inlineStr">
         <is>
-          <t>STEP 1: Flag Marketing Employee Visits (All Sites)</t>
+          <t>STEP 1: Flag Group Functions Employee Visits (All Sites)</t>
         </is>
       </c>
       <c r="B4" s="4" t="n"/>
@@ -2154,7 +2163,7 @@
       </c>
       <c r="B6" s="7" t="inlineStr">
         <is>
-          <t>Marketing</t>
+          <t>Group Functions</t>
         </is>
       </c>
       <c r="C6" s="7" t="inlineStr">
@@ -2201,7 +2210,7 @@
       </c>
       <c r="B7" s="7" t="inlineStr">
         <is>
-          <t>Marketing</t>
+          <t>Group Functions</t>
         </is>
       </c>
       <c r="C7" s="7" t="inlineStr">
@@ -2248,7 +2257,7 @@
       </c>
       <c r="B8" s="7" t="inlineStr">
         <is>
-          <t>Marketing</t>
+          <t>Group Functions</t>
         </is>
       </c>
       <c r="C8" s="7" t="inlineStr">
@@ -2295,7 +2304,7 @@
       </c>
       <c r="B9" s="7" t="inlineStr">
         <is>
-          <t>Marketing</t>
+          <t>Group Functions</t>
         </is>
       </c>
       <c r="C9" s="7" t="inlineStr">
@@ -2337,14 +2346,15 @@
     <row r="10">
       <c r="A10" s="17" t="inlineStr">
         <is>
-          <t>Note: E002 (Sales) and E004 (Engineering) filtered out - not Marketing</t>
-        </is>
-      </c>
-    </row>
+          <t>Note: E002 (GWM) and E004 (IB) filtered out - not Group Functions</t>
+        </is>
+      </c>
+    </row>
+    <row r="11"/>
     <row r="12">
       <c r="A12" s="13" t="inlineStr">
         <is>
-          <t>STEP 2: Deduplicate Marketing Employees</t>
+          <t>STEP 2: Deduplicate Group Functions Employees</t>
         </is>
       </c>
       <c r="B12" s="4" t="n"/>
@@ -2506,6 +2516,7 @@
         </is>
       </c>
     </row>
+    <row r="17"/>
     <row r="18">
       <c r="A18" s="14" t="inlineStr">
         <is>
@@ -2536,7 +2547,7 @@
       </c>
       <c r="C19" s="6" t="inlineStr">
         <is>
-          <t>% of Marketing (5K)</t>
+          <t>% of Group Functions (5K)</t>
         </is>
       </c>
       <c r="D19" s="6" t="inlineStr">
@@ -2658,10 +2669,11 @@
         </is>
       </c>
     </row>
+    <row r="24"/>
     <row r="25">
       <c r="A25" s="16" t="inlineStr">
         <is>
-          <t>KEY INSIGHT: 3 Marketing employees engaged (0.06% of 5,000 Marketing division)</t>
+          <t>KEY INSIGHT: 3 Group Functions employees engaged (0.06% of 5,000 Group Functions division)</t>
         </is>
       </c>
     </row>
@@ -2709,7 +2721,7 @@
     <row r="1">
       <c r="A1" s="10" t="inlineStr">
         <is>
-          <t>SCENARIO 3: Combined Filter - 'News &amp; Events' + 'Marketing'</t>
+          <t>SCENARIO 3: Combined Filter - 'News &amp; Events' + 'Group Functions'</t>
         </is>
       </c>
       <c r="B1" s="4" t="n"/>
@@ -2726,14 +2738,15 @@
     <row r="2">
       <c r="A2" s="11" t="inlineStr">
         <is>
-          <t>Business Question: What % of Marketing engaged with News &amp; Events?</t>
-        </is>
-      </c>
-    </row>
+          <t>Business Question: What % of Group Functions engaged with News &amp; Events?</t>
+        </is>
+      </c>
+    </row>
+    <row r="3"/>
     <row r="4">
       <c r="A4" s="14" t="inlineStr">
         <is>
-          <t>FINAL RESULTS (Marketing employees who visited News &amp; Events)</t>
+          <t>FINAL RESULTS (Group Functions employees who visited News &amp; Events)</t>
         </is>
       </c>
       <c r="B4" s="4" t="n"/>
@@ -2760,7 +2773,7 @@
       </c>
       <c r="C5" s="6" t="inlineStr">
         <is>
-          <t>% of Marketing</t>
+          <t>% of Group Functions</t>
         </is>
       </c>
       <c r="D5" s="6" t="inlineStr">
@@ -2907,10 +2920,11 @@
         </is>
       </c>
     </row>
+    <row r="10"/>
     <row r="11">
       <c r="A11" s="11" t="inlineStr">
         <is>
-          <t>Employees: E001 John, E003 Michael, E005 Carlos (all Marketing, all visited News &amp; Events)</t>
+          <t>Employees: E001 John, E003 Michael, E005 Carlos (all Group Functions, all visited News &amp; Events)</t>
         </is>
       </c>
     </row>
@@ -2963,6 +2977,7 @@
       <c r="G1" s="4" t="n"/>
       <c r="H1" s="5" t="n"/>
     </row>
+    <row r="2"/>
     <row r="3">
       <c r="A3" s="6" t="inlineStr">
         <is>
@@ -3055,7 +3070,7 @@
       </c>
       <c r="B5" s="7" t="inlineStr">
         <is>
-          <t>Marketing</t>
+          <t>Group Functions</t>
         </is>
       </c>
       <c r="C5" s="18" t="inlineStr">
@@ -3131,6 +3146,7 @@
         </is>
       </c>
     </row>
+    <row r="7"/>
     <row r="8">
       <c r="A8" s="19" t="inlineStr">
         <is>

</xml_diff>